<commit_message>
Adding json output functionalit - needs some work, see comments in dashboard_data_icca_to_json nearly there!
</commit_message>
<xml_diff>
--- a/iicudash/COVID_interventions_attributes.xlsx
+++ b/iicudash/COVID_interventions_attributes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="26835" windowHeight="10185"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="26835" windowHeight="10185" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PtAssessment" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="74">
   <si>
     <t>Weight (Admission)</t>
   </si>
@@ -226,6 +226,18 @@
   </si>
   <si>
     <t>Positive end expiratory pressure (observable entity)</t>
+  </si>
+  <si>
+    <t>vname</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Height</t>
   </si>
 </sst>
 </file>
@@ -581,10 +593,422 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="G1:H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>3454</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1">
+        <v>16591</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="1">
+        <v>890</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>3386</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1">
+        <v>20260</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="1">
+        <v>710</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3391</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5390</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1">
+        <v>79</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2199</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="1">
+        <v>440</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="1">
+        <v>989</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>3394</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="1">
+        <v>20082</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1218</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>3394</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="1">
+        <v>20083</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="1">
+        <v>220</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3422</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="1">
+        <v>6449</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="1">
+        <v>823</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>3448</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3926</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="1">
+        <v>969</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>3802</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="1">
+        <v>15302</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="1">
+        <v>959</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>3424</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="1">
+        <v>3378</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="1">
+        <v>927</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>3423</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="1">
+        <v>16177</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="1">
+        <v>616</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>3231</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="1">
+        <v>19522</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1081</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>1980</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="1">
+        <v>19138</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1060</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>3036</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="1">
+        <v>4620</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="1">
+        <v>985</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G1" sqref="G1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,7 +1018,7 @@
     <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
@@ -613,329 +1037,14 @@
       <c r="F1" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>3454</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="1">
-        <v>16591</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="1">
-        <v>890</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>3386</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="1">
-        <v>20260</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="1">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3391</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="1">
-        <v>5390</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="1">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>2199</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="1">
-        <v>440</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="1">
-        <v>989</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>3394</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="1">
-        <v>20082</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1218</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>3394</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="1">
-        <v>20083</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="1">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>3422</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="1">
-        <v>6449</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="1">
-        <v>823</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>3448</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="1">
-        <v>3926</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="1">
-        <v>969</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>3802</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="1">
-        <v>15302</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="1">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>3424</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="1">
-        <v>3378</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="1">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>3423</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="1">
-        <v>16177</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="1">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>3231</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="1">
-        <v>19522</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" s="1">
-        <v>1081</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>1980</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="1">
-        <v>19138</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" s="1">
-        <v>1060</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>3036</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="1">
-        <v>4620</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F15" s="1">
-        <v>985</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="4" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>3368</v>
       </c>
@@ -954,8 +1063,14 @@
       <c r="F2" s="3">
         <v>1128</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>4615</v>
       </c>
@@ -974,8 +1089,14 @@
       <c r="F3" s="1">
         <v>1354</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>8917</v>
       </c>
@@ -994,8 +1115,14 @@
       <c r="F4" s="1">
         <v>1352</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2110</v>
       </c>
@@ -1014,8 +1141,14 @@
       <c r="F5" s="1">
         <v>1352</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>10098</v>
       </c>
@@ -1034,8 +1167,14 @@
       <c r="F6" s="1">
         <v>1350</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2714</v>
       </c>
@@ -1054,8 +1193,14 @@
       <c r="F7" s="1">
         <v>1137</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>3368</v>
       </c>
@@ -1074,8 +1219,14 @@
       <c r="F8" s="1">
         <v>1128</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2377</v>
       </c>
@@ -1094,8 +1245,14 @@
       <c r="F9" s="1">
         <v>330</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2079</v>
       </c>
@@ -1114,8 +1271,14 @@
       <c r="F10" s="1">
         <v>314</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2631</v>
       </c>
@@ -1134,8 +1297,14 @@
       <c r="F11" s="1">
         <v>1389</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2134</v>
       </c>
@@ -1153,6 +1322,12 @@
       </c>
       <c r="F12" s="1">
         <v>1385</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1163,10 +1338,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:F6"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1174,9 +1349,10 @@
     <col min="1" max="4" width="15.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
@@ -1195,8 +1371,14 @@
       <c r="F1" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>22542</v>
       </c>
@@ -1215,8 +1397,14 @@
       <c r="F2" s="3">
         <v>1403</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>807</v>
       </c>
@@ -1235,8 +1423,14 @@
       <c r="F3" s="1">
         <v>1403</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>19699</v>
       </c>
@@ -1255,8 +1449,14 @@
       <c r="F4" s="1">
         <v>1404</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>756</v>
       </c>
@@ -1275,8 +1475,14 @@
       <c r="F5" s="1">
         <v>1405</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4790</v>
       </c>
@@ -1294,6 +1500,12 @@
       </c>
       <c r="F6" s="1">
         <v>1270</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Functional json compiling patient data with schema and previous values. Need to refactor, and styling and increase number of variables in the excel files. Also missing functions to produce derived variables.
</commit_message>
<xml_diff>
--- a/iicudash/COVID_interventions_attributes.xlsx
+++ b/iicudash/COVID_interventions_attributes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="26835" windowHeight="10185" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="26835" windowHeight="10185"/>
   </bookViews>
   <sheets>
     <sheet name="PtAssessment" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="75">
   <si>
     <t>Weight (Admission)</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>Height</t>
+  </si>
+  <si>
+    <t>VT/kg</t>
   </si>
 </sst>
 </file>
@@ -595,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="G1:H1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,7 +792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>3422</v>
       </c>
@@ -809,7 +812,7 @@
         <v>823</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1007,7 +1010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:H1"/>
     </sheetView>
   </sheetViews>
@@ -1341,7 +1344,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1450,7 +1453,7 @@
         <v>1404</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H4">
         <v>0</v>

</xml_diff>

<commit_message>
Refactored and fixed bug: now taking record value that maximises chartTime and only considering priority in cases of duplication.
</commit_message>
<xml_diff>
--- a/iicudash/COVID_interventions_attributes.xlsx
+++ b/iicudash/COVID_interventions_attributes.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="26835" windowHeight="10185"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="26835" windowHeight="10185" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PtAssessment" sheetId="2" r:id="rId1"/>
     <sheet name="PtDemographic" sheetId="4" r:id="rId2"/>
-    <sheet name="PtLabresult" sheetId="5" r:id="rId3"/>
+    <sheet name="PtLabResult" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -598,7 +598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -1343,7 +1343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Introduced choice of valueNumber and valueString to be specified in excel sheets.
</commit_message>
<xml_diff>
--- a/iicudash/COVID_interventions_attributes.xlsx
+++ b/iicudash/COVID_interventions_attributes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="26835" windowHeight="10185" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="26835" windowHeight="10185" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PtAssessment" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="78">
   <si>
     <t>Weight (Admission)</t>
   </si>
@@ -241,6 +241,15 @@
   </si>
   <si>
     <t>VT/kg</t>
+  </si>
+  <si>
+    <t>column</t>
+  </si>
+  <si>
+    <t>valueNumber</t>
+  </si>
+  <si>
+    <t>valueString</t>
   </si>
 </sst>
 </file>
@@ -596,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,9 +617,10 @@
     <col min="5" max="5" width="25.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="23.5703125" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
@@ -635,8 +645,11 @@
       <c r="H1" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I1" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>3454</v>
       </c>
@@ -661,8 +674,11 @@
       <c r="H2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="I2" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>3386</v>
       </c>
@@ -687,8 +703,11 @@
       <c r="H3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="I3" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3391</v>
       </c>
@@ -713,8 +732,11 @@
       <c r="H4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="I4" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2199</v>
       </c>
@@ -739,8 +761,11 @@
       <c r="H5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="I5" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3394</v>
       </c>
@@ -765,8 +790,11 @@
       <c r="H6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="I6" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3394</v>
       </c>
@@ -791,8 +819,11 @@
       <c r="H7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="I7" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>3422</v>
       </c>
@@ -817,8 +848,11 @@
       <c r="H8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I8" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>3448</v>
       </c>
@@ -843,8 +877,11 @@
       <c r="H9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I9" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>3802</v>
       </c>
@@ -869,8 +906,11 @@
       <c r="H10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I10" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>3424</v>
       </c>
@@ -895,8 +935,11 @@
       <c r="H11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="I11" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>3423</v>
       </c>
@@ -921,8 +964,11 @@
       <c r="H12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I12" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>3231</v>
       </c>
@@ -947,8 +993,11 @@
       <c r="H13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I13" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1980</v>
       </c>
@@ -973,8 +1022,11 @@
       <c r="H14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I14" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>3036</v>
       </c>
@@ -998,6 +1050,9 @@
       </c>
       <c r="H15">
         <v>0</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1008,10 +1063,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,9 +1074,10 @@
     <col min="1" max="4" width="15.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
@@ -1046,8 +1102,11 @@
       <c r="H1" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I1" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>3368</v>
       </c>
@@ -1072,8 +1131,11 @@
       <c r="H2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I2" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>4615</v>
       </c>
@@ -1098,8 +1160,11 @@
       <c r="H3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I3" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>8917</v>
       </c>
@@ -1124,8 +1189,11 @@
       <c r="H4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I4" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2110</v>
       </c>
@@ -1150,8 +1218,11 @@
       <c r="H5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I5" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>10098</v>
       </c>
@@ -1176,8 +1247,11 @@
       <c r="H6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2714</v>
       </c>
@@ -1202,8 +1276,11 @@
       <c r="H7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I7" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>3368</v>
       </c>
@@ -1228,8 +1305,11 @@
       <c r="H8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I8" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2377</v>
       </c>
@@ -1254,8 +1334,11 @@
       <c r="H9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I9" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2079</v>
       </c>
@@ -1280,8 +1363,11 @@
       <c r="H10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2631</v>
       </c>
@@ -1306,8 +1392,11 @@
       <c r="H11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I11" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2134</v>
       </c>
@@ -1332,6 +1421,18 @@
       <c r="H12">
         <v>0</v>
       </c>
+      <c r="I12" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1341,10 +1442,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1353,9 +1454,10 @@
     <col min="5" max="5" width="25.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="22.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
@@ -1380,8 +1482,11 @@
       <c r="H1" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I1" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>22542</v>
       </c>
@@ -1406,8 +1511,11 @@
       <c r="H2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I2" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>807</v>
       </c>
@@ -1432,8 +1540,11 @@
       <c r="H3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I3" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>19699</v>
       </c>
@@ -1458,8 +1569,11 @@
       <c r="H4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I4" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>756</v>
       </c>
@@ -1484,8 +1598,11 @@
       <c r="H5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I5" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4790</v>
       </c>
@@ -1509,6 +1626,9 @@
       </c>
       <c r="H6">
         <v>0</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>